<commit_message>
movement is working now
</commit_message>
<xml_diff>
--- a/Data/Level1.xlsx
+++ b/Data/Level1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAE\Semester2\Programming4\GameEngine\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8506D98-DC51-45BE-879B-EBB3BFB4D188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386D7494-31C4-4F50-90EF-914A37E61642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1584" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2016" yWindow="2172" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Level1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="12">
   <si>
     <t>P</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>BBL</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>_</t>
   </si>
 </sst>
 </file>
@@ -893,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1468,6 +1474,100 @@
         <v>2</v>
       </c>
     </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>